<commit_message>
cleaned up scripts file structure
</commit_message>
<xml_diff>
--- a/Data Analysis/Reel Together Evaluation Form.xlsx
+++ b/Data Analysis/Reel Together Evaluation Form.xlsx
@@ -1,40 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Documents\University\Year 3\Final-Year-Project\Data Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2728E26F-BD1A-4CAD-BD64-990CEEF14483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B34F28-BC1A-463A-8BF1-42F182C25AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="17" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="SUS" sheetId="2" r:id="rId2"/>
-    <sheet name="SUS - Feedback" sheetId="14" r:id="rId3"/>
-    <sheet name="GUESS - Usability Playability" sheetId="3" r:id="rId4"/>
-    <sheet name="GUESS - UP - Feedback" sheetId="15" r:id="rId5"/>
-    <sheet name="GUESS - Narratives" sheetId="4" r:id="rId6"/>
-    <sheet name="GUESS - Narrative Feedback" sheetId="16" r:id="rId7"/>
-    <sheet name="GUESS - Play Engrossment" sheetId="5" r:id="rId8"/>
-    <sheet name="GUESS - Engrossment Feedback" sheetId="17" r:id="rId9"/>
-    <sheet name="GUESS - Enjoyment" sheetId="6" r:id="rId10"/>
-    <sheet name="GUESS - Enjoyment Feedback" sheetId="18" r:id="rId11"/>
-    <sheet name="GUESS - Creative Freedom" sheetId="7" r:id="rId12"/>
-    <sheet name="GUESS - Creative free Feedback" sheetId="19" r:id="rId13"/>
-    <sheet name="GUESS - Audio Aesthetics " sheetId="8" r:id="rId14"/>
-    <sheet name="GUESS - Audio Feedback" sheetId="20" r:id="rId15"/>
-    <sheet name="GUESS - Personal Gratification" sheetId="9" r:id="rId16"/>
-    <sheet name="GUESS - Gratification Feedback" sheetId="21" r:id="rId17"/>
-    <sheet name="GUESS - Social Connectivity" sheetId="12" r:id="rId18"/>
-    <sheet name="GUESS - Social Feedback" sheetId="22" r:id="rId19"/>
-    <sheet name="GUESS - Visual Aesthetics" sheetId="13" r:id="rId20"/>
-    <sheet name="GUESS - Visual Feedback" sheetId="23" r:id="rId21"/>
-    <sheet name="Global Feedback" sheetId="24" r:id="rId22"/>
+    <sheet name="SUS" sheetId="2" r:id="rId1"/>
+    <sheet name="SUS - Feedback" sheetId="14" r:id="rId2"/>
+    <sheet name="GUESS - Usability Playability" sheetId="3" r:id="rId3"/>
+    <sheet name="GUESS - UP - Feedback" sheetId="15" r:id="rId4"/>
+    <sheet name="GUESS - Narratives" sheetId="4" r:id="rId5"/>
+    <sheet name="GUESS - Narrative Feedback" sheetId="16" r:id="rId6"/>
+    <sheet name="GUESS - Play Engrossment" sheetId="5" r:id="rId7"/>
+    <sheet name="GUESS - Engrossment Feedback" sheetId="17" r:id="rId8"/>
+    <sheet name="GUESS - Enjoyment" sheetId="6" r:id="rId9"/>
+    <sheet name="GUESS - Enjoyment Feedback" sheetId="18" r:id="rId10"/>
+    <sheet name="GUESS - Creative Freedom" sheetId="7" r:id="rId11"/>
+    <sheet name="GUESS - Creative free Feedback" sheetId="19" r:id="rId12"/>
+    <sheet name="GUESS - Audio Aesthetics " sheetId="8" r:id="rId13"/>
+    <sheet name="GUESS - Audio Feedback" sheetId="20" r:id="rId14"/>
+    <sheet name="GUESS - Personal Gratification" sheetId="9" r:id="rId15"/>
+    <sheet name="GUESS - Gratification Feedback" sheetId="21" r:id="rId16"/>
+    <sheet name="GUESS - Social Connectivity" sheetId="12" r:id="rId17"/>
+    <sheet name="GUESS - Social Feedback" sheetId="22" r:id="rId18"/>
+    <sheet name="GUESS - Visual Aesthetics" sheetId="13" r:id="rId19"/>
+    <sheet name="GUESS - Visual Feedback" sheetId="23" r:id="rId20"/>
+    <sheet name="Global Feedback" sheetId="24" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -57,54 +56,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="100">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>What is your BCU email address (it will only be used as ID. It will not be published)</t>
-  </si>
-  <si>
     <t>Feel free to use this section to expand on any of your answers</t>
   </si>
   <si>
-    <t>Please rate your confidence in using etee vr controllers.Confidence</t>
-  </si>
-  <si>
     <t>If you have any other feedback feel free to use this section</t>
   </si>
   <si>
-    <t>Confident</t>
-  </si>
-  <si>
-    <t>Very Confident</t>
-  </si>
-  <si>
-    <t>Morgan.Lowe@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Morgan Lowe</t>
-  </si>
-  <si>
-    <t>Unconfident</t>
-  </si>
-  <si>
     <t>The controllers sometimes felt to desync or change in input</t>
-  </si>
-  <si>
-    <t>Sean.Andrews2@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Sean Thomas Andrews</t>
-  </si>
-  <si>
-    <t>sean.andrews2@mail.bcu.ac.uk</t>
   </si>
   <si>
     <t xml:space="preserve">Amazing game James, loved every aspect of the game, even the hat customisation, absolutely out done yourself </t>
@@ -141,45 +104,12 @@
     <t>Very easy to use</t>
   </si>
   <si>
-    <t>Remari.Burrell@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Remari Burrell</t>
-  </si>
-  <si>
-    <t>Remari.burrell@mail.bcu.ac.uk</t>
-  </si>
-  <si>
     <t xml:space="preserve">This game was amazing. Would definitely recommend </t>
   </si>
   <si>
-    <t>Ben.Brick@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Ben Brick</t>
-  </si>
-  <si>
     <t>My play through experience while fun consisted of a few bugs one of which stopped my progression but it was funny</t>
   </si>
   <si>
-    <t>Joshua.Evans5@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Joshua Evans</t>
-  </si>
-  <si>
-    <t>Joshua.evans5@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Agnes.Eriksson@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Agnes Eriksson</t>
-  </si>
-  <si>
-    <t>agnes.eriksson@mail.bcu.ac.uk</t>
-  </si>
-  <si>
     <t xml:space="preserve">It took a while to understand how the controllers worked and I had to squeeze pretty hard </t>
   </si>
   <si>
@@ -192,96 +122,27 @@
     <t xml:space="preserve">I really liked the hat selection </t>
   </si>
   <si>
-    <t>William.Harper@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>William Harper</t>
-  </si>
-  <si>
-    <t>william.harper@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Vennce.Bravo@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Vennce Bravo</t>
-  </si>
-  <si>
-    <t>vennce.bravo@mail.bcu.ac.uk</t>
-  </si>
-  <si>
     <t>The game was really fun to play both in multiplayer and single player. I really enjoyed how simple yet intuitive the controls were. The controllers themselves was really well implemented into the game.</t>
   </si>
   <si>
-    <t>Khai.Ailyan@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Khai Ailyan</t>
-  </si>
-  <si>
-    <t>Khai.ailyan@mail.bcu.ac.uk</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Very Unconfident</t>
-  </si>
-  <si>
-    <t>Henry.Cutts@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Henry Cutts</t>
-  </si>
-  <si>
-    <t>henry.cutts@mail.bcu.ac.uk</t>
-  </si>
-  <si>
     <t xml:space="preserve">Inconsistency - controllers were low battery which induced errors in gesture reading </t>
   </si>
   <si>
     <t>Low battery induces many errors</t>
   </si>
   <si>
-    <t>oliwier.gregorczyk@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Oliwier Gregorczyk</t>
-  </si>
-  <si>
-    <t>Oliwier Gregorczyk@mail.bcu.ac.uk</t>
-  </si>
-  <si>
     <t xml:space="preserve">Controller positing was iffy but other than that it was okay </t>
   </si>
   <si>
-    <t>jason.robb@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Jason Robb</t>
-  </si>
-  <si>
     <t>I wouldn’t understand how to use the controllers without some sort of manual first</t>
   </si>
   <si>
     <t>Did not play long enough to feel these emotions</t>
   </si>
   <si>
-    <t>James.Bland@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>James Bland</t>
-  </si>
-  <si>
-    <t>Oliver.Byrne3@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Dylan.Furniss@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Dylan Furniss</t>
-  </si>
-  <si>
     <t>The simplicity of the system is great, but the feedback it gives to the player in what movement is necessary to achieve any goal is incredibly inconsistent, as the movements are often too precise.</t>
   </si>
   <si>
@@ -294,55 +155,10 @@
     <t xml:space="preserve">The multilayer mode is very competitive. </t>
   </si>
   <si>
-    <t>Tyler.Mills@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Tyler Mills</t>
-  </si>
-  <si>
-    <t>tyler.mills@mail.bcu.ac.uk</t>
-  </si>
-  <si>
     <t>The controls were simple but sometimes the controllers would go out if sync</t>
   </si>
   <si>
-    <t>Temujin.Tansey@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Temujin Tansey</t>
-  </si>
-  <si>
-    <t>temujin.tansey@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Jack.Longmore@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Jack Longmore</t>
-  </si>
-  <si>
-    <t>jack.longmore@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Cameron.Binning@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>Cameron Binning</t>
-  </si>
-  <si>
-    <t>Cameron.binning@mail.bcu.ac.uk</t>
-  </si>
-  <si>
-    <t>anonymous</t>
-  </si>
-  <si>
-    <t>Erin-mcgarry@outlook.com</t>
-  </si>
-  <si>
     <t>I really enjoyed the game and asked to replay it several times</t>
-  </si>
-  <si>
-    <t>toby.s.fisher@outlook.com</t>
   </si>
   <si>
     <t>Loved the game</t>
@@ -668,7 +484,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="120">
+  <dxfs count="115">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -2393,21 +2209,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2422,359 +2223,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:E21" totalsRowShown="0">
-  <autoFilter ref="A1:E21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="119">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="id"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="118">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="responder"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="117">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="responderName"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="What is your BCU email address (it will only be used as ID. It will not be published)" dataDxfId="116">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="r32bc8cf535cb4e6eab018064e078f2c4"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="271" xr3:uid="{00000000-0010-0000-0000-00000F010000}" name="Please rate your confidence in using etee vr controllers.Confidence" dataDxfId="115">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="r0e1a2eb4f0864b19ad631ceb900b6b3b"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-  <extLst>
-    <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{839C7E11-91E4-4DBD-9C5D-0DEA604FA9AC}">
-      <xlmsforms:msForm id="VeArfoqCI0W15bd62ZOXhU2JS25C7mJDogalqQr6cuNUMkNPVk5RT1ROUzBGUDlLMUhTQVQ4OUNRNC4u" isFormConnected="1" maxResponseId="24" latestEventMarker="1">
-        <xlmsforms:syncedQuestionId>id</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>startDate</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>submitDate</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>responder</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>responderName</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>totalScore</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>quizFeedback</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>releaseDate</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r32bc8cf535cb4e6eab018064e078f2c4</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r32bc8cf535cb4e6eab018064e078f2c4-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r32bc8cf535cb4e6eab018064e078f2c4-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r636b0079b22e4ff4837d4615995b0ac8</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r636b0079b22e4ff4837d4615995b0ac8-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r636b0079b22e4ff4837d4615995b0ac8-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r8c42d03813eb4e66af213c69a18b6b66</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r8c42d03813eb4e66af213c69a18b6b66-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r8c42d03813eb4e66af213c69a18b6b66-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rd37d7a0190ed440dbe24ed7b0a236df9-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rd37d7a0190ed440dbe24ed7b0a236df9-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r68923229d9b048b0b79e7daa915a1cfc</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r68923229d9b048b0b79e7daa915a1cfc-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r68923229d9b048b0b79e7daa915a1cfc-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r42f14e97dcc647be96b8a4983efa6c00</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r42f14e97dcc647be96b8a4983efa6c00-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r42f14e97dcc647be96b8a4983efa6c00-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r2ed2668843a14b7a9b0ddbbffe9c2892</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r2ed2668843a14b7a9b0ddbbffe9c2892-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r2ed2668843a14b7a9b0ddbbffe9c2892-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r982979ed7c2d42f8adb3e3c923c7fc31</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r982979ed7c2d42f8adb3e3c923c7fc31-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r982979ed7c2d42f8adb3e3c923c7fc31-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb2f40553a83d43ca93a5bada5be38ee6</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb2f40553a83d43ca93a5bada5be38ee6-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb2f40553a83d43ca93a5bada5be38ee6-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc7dc82887f65466897be36cab6e7707b</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc7dc82887f65466897be36cab6e7707b-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc7dc82887f65466897be36cab6e7707b-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ree8bca491d214a4798378961c76d79bc</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ree8bca491d214a4798378961c76d79bc-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ree8bca491d214a4798378961c76d79bc-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r81902af28ae14dd19e0b91cf4b970e94</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r81902af28ae14dd19e0b91cf4b970e94-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r81902af28ae14dd19e0b91cf4b970e94-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r444b4e3844ba44b3b9460763a01229f3</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r444b4e3844ba44b3b9460763a01229f3-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r444b4e3844ba44b3b9460763a01229f3-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfa8c4d9d917e4adc8f48b0b7f36d74f7</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfa8c4d9d917e4adc8f48b0b7f36d74f7-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfa8c4d9d917e4adc8f48b0b7f36d74f7-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rd352e83b7ecb4a479effbbd74377d39b</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rd352e83b7ecb4a479effbbd74377d39b-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rd352e83b7ecb4a479effbbd74377d39b-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r041e10bb033e4f2f9cb95a72b1bfc0e2</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r041e10bb033e4f2f9cb95a72b1bfc0e2-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r041e10bb033e4f2f9cb95a72b1bfc0e2-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r4775588bfb2f433282fc2eaf752c64e3</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r4775588bfb2f433282fc2eaf752c64e3-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r4775588bfb2f433282fc2eaf752c64e3-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r867977eaf1eb4528a9b8a8fe1395fc79-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r867977eaf1eb4528a9b8a8fe1395fc79-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra3207a7582be43f0af056f797aaa02f0</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra3207a7582be43f0af056f797aaa02f0-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra3207a7582be43f0af056f797aaa02f0-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb5caa0bf35ac4d4bad8a9487a4ef1b5d</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb5caa0bf35ac4d4bad8a9487a4ef1b5d-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb5caa0bf35ac4d4bad8a9487a4ef1b5d-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7221fc36469442528e3f620bee129653</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7221fc36469442528e3f620bee129653-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7221fc36469442528e3f620bee129653-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r179eb94f6cdc4ed7bab9fd9362f80ab3</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r179eb94f6cdc4ed7bab9fd9362f80ab3-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r179eb94f6cdc4ed7bab9fd9362f80ab3-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1ab2badf69c0443e9b77d144f7b4c29b</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1ab2badf69c0443e9b77d144f7b4c29b-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1ab2badf69c0443e9b77d144f7b4c29b-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra3b352c501a148e7a850b2b58f867c12</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra3b352c501a148e7a850b2b58f867c12-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra3b352c501a148e7a850b2b58f867c12-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb2d1a2b8720a4e1c819002997866d8cf</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb2d1a2b8720a4e1c819002997866d8cf-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb2d1a2b8720a4e1c819002997866d8cf-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r9298f4b349b640e999e379d43e2f30d0</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r9298f4b349b640e999e379d43e2f30d0-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r9298f4b349b640e999e379d43e2f30d0-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1fbb29ac3aa345008f94c7ca85c4b975</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1fbb29ac3aa345008f94c7ca85c4b975-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1fbb29ac3aa345008f94c7ca85c4b975-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>re6356ab04e4d477bbb6cca049f53a864</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>re6356ab04e4d477bbb6cca049f53a864-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>re6356ab04e4d477bbb6cca049f53a864-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r35d1309d281f46249e90f6bfad59724c</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r35d1309d281f46249e90f6bfad59724c-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r35d1309d281f46249e90f6bfad59724c-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r52fe507fc0b64b62904f030384b43c40</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r52fe507fc0b64b62904f030384b43c40-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r52fe507fc0b64b62904f030384b43c40-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1d449bfda8254117a70d455fc6425425-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1d449bfda8254117a70d455fc6425425-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf5eee8b1a5654d24b1e7633e368832fc</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf5eee8b1a5654d24b1e7633e368832fc-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf5eee8b1a5654d24b1e7633e368832fc-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1dfab59638184a03b2d01896cc5e9806</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1dfab59638184a03b2d01896cc5e9806-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r1dfab59638184a03b2d01896cc5e9806-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r3f7645810ebc4678b27b41ef585f4ae2</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r3f7645810ebc4678b27b41ef585f4ae2-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r3f7645810ebc4678b27b41ef585f4ae2-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r86ee354844c94546877f4f1d3a6090b5</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r86ee354844c94546877f4f1d3a6090b5-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r86ee354844c94546877f4f1d3a6090b5-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf6b2dca391c148e3bd918750a10e5453</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf6b2dca391c148e3bd918750a10e5453-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf6b2dca391c148e3bd918750a10e5453-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rec3092c92d4f469da08bd88fcf2dcb40</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rec3092c92d4f469da08bd88fcf2dcb40-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rec3092c92d4f469da08bd88fcf2dcb40-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rcea98e278733408389b7bbda929c02f5</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rcea98e278733408389b7bbda929c02f5-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rcea98e278733408389b7bbda929c02f5-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r3d4ef95be30842e3b1db75b315cd9b20</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r3d4ef95be30842e3b1db75b315cd9b20-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r3d4ef95be30842e3b1db75b315cd9b20-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r97acdad7c6404945ae03fb584b4b3b81-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r97acdad7c6404945ae03fb584b4b3b81-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r549e5744b793421e9c89eb82d58c2ae9</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r549e5744b793421e9c89eb82d58c2ae9-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r549e5744b793421e9c89eb82d58c2ae9-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rca52702d841a4d40ae9b1637ed2db434</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rca52702d841a4d40ae9b1637ed2db434-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rca52702d841a4d40ae9b1637ed2db434-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rbc2f2dcacc7a4a6e85c88bcb00fc318f</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rbc2f2dcacc7a4a6e85c88bcb00fc318f-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rbc2f2dcacc7a4a6e85c88bcb00fc318f-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7fd24b13308d49f4a6846414801210f4</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7fd24b13308d49f4a6846414801210f4-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7fd24b13308d49f4a6846414801210f4-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc80fef3a42864cca8467656466eb4147</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc80fef3a42864cca8467656466eb4147-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc80fef3a42864cca8467656466eb4147-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r6ba18ed2a5e9427f9d9b3e1543132569</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r6ba18ed2a5e9427f9d9b3e1543132569-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r6ba18ed2a5e9427f9d9b3e1543132569-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r65e0e187139548979276238b7283d0cc</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r65e0e187139548979276238b7283d0cc-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r65e0e187139548979276238b7283d0cc-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r81951a6c99724bb3b2c722af019406a7</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r81951a6c99724bb3b2c722af019406a7-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r81951a6c99724bb3b2c722af019406a7-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb19ce0e9afc549cdb9e888febdc2af10</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb19ce0e9afc549cdb9e888febdc2af10-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb19ce0e9afc549cdb9e888febdc2af10-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r72685bec4cff404cb07b31ef64f219e6-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r72685bec4cff404cb07b31ef64f219e6-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf9ed65b05d5f4f9190f216744b7047aa</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf9ed65b05d5f4f9190f216744b7047aa-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf9ed65b05d5f4f9190f216744b7047aa-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra9e6dd7a534747cdba69c7b5eed1e343</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra9e6dd7a534747cdba69c7b5eed1e343-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra9e6dd7a534747cdba69c7b5eed1e343-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r620493d9403549588447bdcfe3bab209</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r620493d9403549588447bdcfe3bab209-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r620493d9403549588447bdcfe3bab209-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7f2f6246ea2c46f7a90f9ed085299415</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7f2f6246ea2c46f7a90f9ed085299415-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7f2f6246ea2c46f7a90f9ed085299415-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r28803b8e786b4aa39b8da99e622d5326</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r28803b8e786b4aa39b8da99e622d5326-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r28803b8e786b4aa39b8da99e622d5326-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r95712de72c014b1ab4a40f05c81f5b54</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r95712de72c014b1ab4a40f05c81f5b54-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r95712de72c014b1ab4a40f05c81f5b54-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra6275b8744c74a29b36bf739450a1ad6-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ra6275b8744c74a29b36bf739450a1ad6-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r2f7ecb0ca8b744a6814a1d9e95789186</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r2f7ecb0ca8b744a6814a1d9e95789186-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r2f7ecb0ca8b744a6814a1d9e95789186-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r35bb671a5a0445f7b61e9dd5dfa6d4f2</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r35bb671a5a0445f7b61e9dd5dfa6d4f2-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r35bb671a5a0445f7b61e9dd5dfa6d4f2-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r8f0d0dfca39d4ad1b0b7ae7244ceb3c2</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r8f0d0dfca39d4ad1b0b7ae7244ceb3c2-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r8f0d0dfca39d4ad1b0b7ae7244ceb3c2-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfdd1b9a416464c4ab02cb7d24331b9c2</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfdd1b9a416464c4ab02cb7d24331b9c2-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfdd1b9a416464c4ab02cb7d24331b9c2-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>re2ef5ff967de42aaa0d305c2d8911880</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>re2ef5ff967de42aaa0d305c2d8911880-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>re2ef5ff967de42aaa0d305c2d8911880-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r59614d04412f42488c46c886c4dc6c47</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r59614d04412f42488c46c886c4dc6c47-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r59614d04412f42488c46c886c4dc6c47-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r85916e0954e6490b976c0ea0b7dc8193</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r85916e0954e6490b976c0ea0b7dc8193-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r85916e0954e6490b976c0ea0b7dc8193-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>raf498b43b3554108944c1de3ae9ac803</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>raf498b43b3554108944c1de3ae9ac803-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>raf498b43b3554108944c1de3ae9ac803-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r10ee3e1873df4e749da72db3699e0b0e-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r10ee3e1873df4e749da72db3699e0b0e-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r3068cfe104924a158b773ab018aaf5ab</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r3068cfe104924a158b773ab018aaf5ab-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r3068cfe104924a158b773ab018aaf5ab-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rd24f0e45d57148669df11ee22cc46b35</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rd24f0e45d57148669df11ee22cc46b35-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rd24f0e45d57148669df11ee22cc46b35-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb062bef5a23c426ab50391394e16208b</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb062bef5a23c426ab50391394e16208b-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb062bef5a23c426ab50391394e16208b-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfd5e982c76b2425c82936d5a11ce4c4a</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfd5e982c76b2425c82936d5a11ce4c4a-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfd5e982c76b2425c82936d5a11ce4c4a-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r747a2248559346c8903d3544d024d6fe</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r747a2248559346c8903d3544d024d6fe-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r747a2248559346c8903d3544d024d6fe-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r5bd29574e6904ca982723312f776bfaf-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r5bd29574e6904ca982723312f776bfaf-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r234c2ae0d15b4a698f3c8a130278152c</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r234c2ae0d15b4a698f3c8a130278152c-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r234c2ae0d15b4a698f3c8a130278152c-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ree4088bd1bb24e448b298ec109a1b990</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ree4088bd1bb24e448b298ec109a1b990-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>ree4088bd1bb24e448b298ec109a1b990-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r0457e1bf8fea4684bd41526566094d13</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r0457e1bf8fea4684bd41526566094d13-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r0457e1bf8fea4684bd41526566094d13-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc95da8680ba24868a83070e8eca2e411</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc95da8680ba24868a83070e8eca2e411-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc95da8680ba24868a83070e8eca2e411-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r18dd9754bf884b17ac33232f045c74e3</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r18dd9754bf884b17ac33232f045c74e3-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r18dd9754bf884b17ac33232f045c74e3-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r5251d288cc6848b4929dcb77ea1bfa40</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r5251d288cc6848b4929dcb77ea1bfa40-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r5251d288cc6848b4929dcb77ea1bfa40-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7a2ee8a40fb9494a999950ae70c6677a</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7a2ee8a40fb9494a999950ae70c6677a-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r7a2ee8a40fb9494a999950ae70c6677a-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfbc6373a6f0345d19f26577340ff751d-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rfbc6373a6f0345d19f26577340ff751d-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r11032a7049ec4591a602ae93ea3c4c2d</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r11032a7049ec4591a602ae93ea3c4c2d-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r11032a7049ec4591a602ae93ea3c4c2d-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r11c92feb3a1c4a40a3a670d0db0813af</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r11c92feb3a1c4a40a3a670d0db0813af-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r11c92feb3a1c4a40a3a670d0db0813af-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r9e1b875ababb44708ee55476f1e8c99d</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r9e1b875ababb44708ee55476f1e8c99d-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r9e1b875ababb44708ee55476f1e8c99d-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc110c1293d204b3bbe4a4dd23b5c41d0</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc110c1293d204b3bbe4a4dd23b5c41d0-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc110c1293d204b3bbe4a4dd23b5c41d0-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rbe2cf382e7bd4d61a1cdf6cb18d6fac3</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rbe2cf382e7bd4d61a1cdf6cb18d6fac3-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rbe2cf382e7bd4d61a1cdf6cb18d6fac3-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r8a226e8f946d4faebfe608007b4b9027-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r8a226e8f946d4faebfe608007b4b9027-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r39429fe5a07146109b938569de2ebed7</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r39429fe5a07146109b938569de2ebed7-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r39429fe5a07146109b938569de2ebed7-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r96d5c1c8a14e4f0da174726af96ad1b2</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r96d5c1c8a14e4f0da174726af96ad1b2-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r96d5c1c8a14e4f0da174726af96ad1b2-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rcf9dfd189ceb41d88fe37745c628cca7</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rcf9dfd189ceb41d88fe37745c628cca7-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rcf9dfd189ceb41d88fe37745c628cca7-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r9ae47c08ec364a9f9a2ddebda648aeae</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r9ae47c08ec364a9f9a2ddebda648aeae-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r9ae47c08ec364a9f9a2ddebda648aeae-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rcbc7a80b9d434b1a99dad3972ed3dab1-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rcbc7a80b9d434b1a99dad3972ed3dab1-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r0e1a2eb4f0864b19ad631ceb900b6b3b</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r0e1a2eb4f0864b19ad631ceb900b6b3b-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r0e1a2eb4f0864b19ad631ceb900b6b3b-Comment</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb85461128db048d987b096c3bbfe918b</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb85461128db048d987b096c3bbfe918b-Score</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rb85461128db048d987b096c3bbfe918b-Comment</xlmsforms:syncedQuestionId>
-      </xlmsforms:msForm>
-    </ext>
-  </extLst>
-</table>
-</file>
-
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{22F2731F-79F9-4D35-988C-57240E4CA413}" name="Table10" displayName="Table10" ref="A1:E21" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A1:E21" xr:uid="{22F2731F-79F9-4D35-988C-57240E4CA413}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7BF06737-6217-431E-8FA9-DDB5C2B94113}" name="Id" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{EBA3BABA-5AE2-4D9D-BBCE-6141DD183049}" name="I find the game supports social interaction (e.g., chat) between players." dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{B524A9A9-58CA-4CD9-9380-2E99EBD28ABC}" name="I like to play this game with other players." dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{BCF2DD92-6C2A-4815-B436-4480B2630347}" name="I am able to play the game with other players if i choose" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{0079DCD0-87B9-45E2-8F0B-40878832F256}" name="I enjoy the social interaction within the game" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5D9257E8-AC6E-40D9-9586-9DF277407EBA}" name="Table11" displayName="Table11" ref="A1:D21" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D21" xr:uid="{5D9257E8-AC6E-40D9-9586-9DF277407EBA}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EF741B5A-C324-4FDB-9878-0F30B6583A68}" name="Id" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{69E0B13F-0CC5-4EF1-87E9-B9E188CA87EB}" name="I enjoy the game's graphics" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{31DF4507-19E6-4CFF-9D18-6C1A0BF5B13E}" name="I think the graphics of the game fit the mood or style of the game" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{46D31FEF-8ABD-48B1-B231-A1036CFC0B18}" name="I think the game is visually appealing" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4471543-8984-40AA-89F7-9709270BE99B}" name="Table2" displayName="Table2" ref="A1:J21" totalsRowShown="0" headerRowDxfId="114" dataDxfId="112" headerRowBorderDxfId="113" tableBorderDxfId="111" totalsRowBorderDxfId="110">
   <autoFilter ref="A1:J21" xr:uid="{C4471543-8984-40AA-89F7-9709270BE99B}"/>
   <tableColumns count="10">
@@ -2793,7 +2241,20 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5D9257E8-AC6E-40D9-9586-9DF277407EBA}" name="Table11" displayName="Table11" ref="A1:D21" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D21" xr:uid="{5D9257E8-AC6E-40D9-9586-9DF277407EBA}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{EF741B5A-C324-4FDB-9878-0F30B6583A68}" name="Id" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{69E0B13F-0CC5-4EF1-87E9-B9E188CA87EB}" name="I enjoy the game's graphics" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{31DF4507-19E6-4CFF-9D18-6C1A0BF5B13E}" name="I think the graphics of the game fit the mood or style of the game" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{46D31FEF-8ABD-48B1-B231-A1036CFC0B18}" name="I think the game is visually appealing" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A7C8ADA1-84D3-478B-B01D-4A29F34CAC60}" name="Table3" displayName="Table3" ref="A1:L21" totalsRowShown="0" headerRowDxfId="99" headerRowBorderDxfId="98" tableBorderDxfId="97" totalsRowBorderDxfId="96">
   <autoFilter ref="A1:L21" xr:uid="{A7C8ADA1-84D3-478B-B01D-4A29F34CAC60}"/>
   <tableColumns count="12">
@@ -2814,7 +2275,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{23FE70E2-BBBA-4B95-82A4-A0A51DEAA706}" name="Table4" displayName="Table4" ref="A1:H21" totalsRowShown="0" headerRowDxfId="83" headerRowBorderDxfId="82" tableBorderDxfId="81" totalsRowBorderDxfId="80">
   <autoFilter ref="A1:H21" xr:uid="{23FE70E2-BBBA-4B95-82A4-A0A51DEAA706}"/>
   <tableColumns count="8">
@@ -2831,7 +2292,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F3C9E107-A74D-4E7A-BF83-5940CAC01565}" name="Table5" displayName="Table5" ref="A1:I21" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <autoFilter ref="A1:I21" xr:uid="{F3C9E107-A74D-4E7A-BF83-5940CAC01565}"/>
   <tableColumns count="9">
@@ -2849,7 +2310,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C6F4D3B4-078E-468D-8909-81EB6FBB1C94}" name="Table6" displayName="Table6" ref="A1:F21" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <autoFilter ref="A1:F21" xr:uid="{C6F4D3B4-078E-468D-8909-81EB6FBB1C94}"/>
   <tableColumns count="6">
@@ -2864,7 +2325,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D8671FFE-1CAD-4FF7-A964-A7FB6AC724CE}" name="Table7" displayName="Table7" ref="A1:H21" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="A1:H21" xr:uid="{D8671FFE-1CAD-4FF7-A964-A7FB6AC724CE}"/>
   <tableColumns count="8">
@@ -2881,7 +2342,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{73BB9AE5-C4C9-4578-93FF-7FFB6E154DAD}" name="Table8" displayName="Table8" ref="A1:E21" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="A1:E21" xr:uid="{73BB9AE5-C4C9-4578-93FF-7FFB6E154DAD}"/>
   <tableColumns count="5">
@@ -2895,7 +2356,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8863303B-C6F0-4B8F-84CD-723797BCBB4D}" name="Table9" displayName="Table9" ref="A1:G21" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="A1:G21" xr:uid="{8863303B-C6F0-4B8F-84CD-723797BCBB4D}"/>
   <tableColumns count="7">
@@ -2906,6 +2367,20 @@
     <tableColumn id="5" xr3:uid="{484A1537-7F63-423C-9DF7-31858D946E97}" name="I am very focused on my own performance while playing the game" dataDxfId="19"/>
     <tableColumn id="6" xr3:uid="{00B23ECE-0AB8-48C8-AE52-6535026323A6}" name="I feel the game constantly motivates me to proceed further to the next stage or level" dataDxfId="18"/>
     <tableColumn id="7" xr3:uid="{F8586636-3840-412F-8853-FAF815D37E6D}" name="I find my skills gradually improve through the course of overcoming the challenges in the game" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{22F2731F-79F9-4D35-988C-57240E4CA413}" name="Table10" displayName="Table10" ref="A1:E21" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:E21" xr:uid="{22F2731F-79F9-4D35-988C-57240E4CA413}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{7BF06737-6217-431E-8FA9-DDB5C2B94113}" name="Id" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{EBA3BABA-5AE2-4D9D-BBCE-6141DD183049}" name="I find the game supports social interaction (e.g., chat) between players." dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{B524A9A9-58CA-4CD9-9380-2E99EBD28ABC}" name="I like to play this game with other players." dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{BCF2DD92-6C2A-4815-B436-4480B2630347}" name="I am able to play the game with other players if i choose" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{0079DCD0-87B9-45E2-8F0B-40878832F256}" name="I enjoy the social interaction within the game" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3207,397 +2682,703 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21EFD8E-1233-4766-ABCE-33EC154D85E9}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView zoomScale="51" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" customWidth="1"/>
-    <col min="6" max="6" width="38.6640625" customWidth="1"/>
-    <col min="7" max="7" width="88.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="75.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="70.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="128.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="78.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="94.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="115.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="79" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="71.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="112.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="180.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="82.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="90.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="29" width="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="255.6640625" customWidth="1"/>
-    <col min="31" max="93" width="20" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="79" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="84" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="182.21875" bestFit="1" customWidth="1"/>
-    <col min="97" max="276" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.88671875" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="75.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="69.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="65.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4">
+        <v>4</v>
+      </c>
+      <c r="H2" s="4">
+        <v>4</v>
+      </c>
+      <c r="I2" s="4">
+        <v>4</v>
+      </c>
+      <c r="J2" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6">
+        <v>5</v>
+      </c>
+      <c r="H3" s="6">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="I3" s="6">
+        <v>5</v>
+      </c>
+      <c r="J3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="I4" s="4">
+        <v>5</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6">
+        <v>4</v>
+      </c>
+      <c r="G5" s="6">
+        <v>4</v>
+      </c>
+      <c r="H5" s="6">
+        <v>4</v>
+      </c>
+      <c r="I5" s="6">
+        <v>4</v>
+      </c>
+      <c r="J5" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>3</v>
+      </c>
+      <c r="I6" s="4">
+        <v>4</v>
+      </c>
+      <c r="J6" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6">
+        <v>4</v>
+      </c>
+      <c r="E7" s="6">
+        <v>4</v>
+      </c>
+      <c r="F7" s="6">
+        <v>3</v>
+      </c>
+      <c r="G7" s="6">
+        <v>4</v>
+      </c>
+      <c r="H7" s="6">
+        <v>3</v>
+      </c>
+      <c r="I7" s="6">
+        <v>4</v>
+      </c>
+      <c r="J7" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>4</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>4</v>
+      </c>
+      <c r="J8" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>5</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>5</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>5</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B11" s="6">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>4</v>
+      </c>
+      <c r="G11" s="6">
+        <v>5</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6">
+        <v>5</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="B12" s="4">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4">
+        <v>4</v>
+      </c>
+      <c r="G12" s="4">
+        <v>5</v>
+      </c>
+      <c r="H12" s="4">
+        <v>2</v>
+      </c>
+      <c r="I12" s="4">
+        <v>4</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="B13" s="6">
+        <v>4</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6">
+        <v>4</v>
+      </c>
+      <c r="F13" s="6">
+        <v>5</v>
+      </c>
+      <c r="G13" s="6">
+        <v>4</v>
+      </c>
+      <c r="H13" s="6">
+        <v>2</v>
+      </c>
+      <c r="I13" s="6">
+        <v>4</v>
+      </c>
+      <c r="J13" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4</v>
+      </c>
+      <c r="G14" s="4">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4">
+        <v>4</v>
+      </c>
+      <c r="I14" s="4">
+        <v>4</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="B15" s="6">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <v>2</v>
+      </c>
+      <c r="E15" s="6">
+        <v>2</v>
+      </c>
+      <c r="F15" s="6">
+        <v>5</v>
+      </c>
+      <c r="G15" s="6">
+        <v>4</v>
+      </c>
+      <c r="H15" s="6">
+        <v>4</v>
+      </c>
+      <c r="I15" s="6">
+        <v>4</v>
+      </c>
+      <c r="J15" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3</v>
+      </c>
+      <c r="F16" s="4">
+        <v>4</v>
+      </c>
+      <c r="G16" s="4">
+        <v>4</v>
+      </c>
+      <c r="H16" s="4">
+        <v>3</v>
+      </c>
+      <c r="I16" s="4">
+        <v>5</v>
+      </c>
+      <c r="J16" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2</v>
+      </c>
+      <c r="E17" s="6">
+        <v>2</v>
+      </c>
+      <c r="F17" s="6">
+        <v>4</v>
+      </c>
+      <c r="G17" s="6">
+        <v>3</v>
+      </c>
+      <c r="H17" s="6">
+        <v>2</v>
+      </c>
+      <c r="I17" s="6">
+        <v>4</v>
+      </c>
+      <c r="J17" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="B18" s="4">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4">
+        <v>4</v>
+      </c>
+      <c r="E18" s="4">
+        <v>5</v>
+      </c>
+      <c r="F18" s="4">
+        <v>3</v>
+      </c>
+      <c r="G18" s="4">
+        <v>4</v>
+      </c>
+      <c r="H18" s="4">
+        <v>3</v>
+      </c>
+      <c r="I18" s="4">
+        <v>3</v>
+      </c>
+      <c r="J18" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="B19" s="6">
+        <v>4</v>
+      </c>
+      <c r="C19" s="6">
+        <v>3</v>
+      </c>
+      <c r="D19" s="6">
+        <v>4</v>
+      </c>
+      <c r="E19" s="6">
+        <v>4</v>
+      </c>
+      <c r="F19" s="6">
+        <v>3</v>
+      </c>
+      <c r="G19" s="6">
+        <v>4</v>
+      </c>
+      <c r="H19" s="6">
+        <v>2</v>
+      </c>
+      <c r="I19" s="6">
+        <v>4</v>
+      </c>
+      <c r="J19" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="B20" s="4">
+        <v>5</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>4</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>4</v>
+      </c>
+      <c r="G20" s="4">
+        <v>4</v>
+      </c>
+      <c r="H20" s="4">
+        <v>2</v>
+      </c>
+      <c r="I20" s="4">
+        <v>4</v>
+      </c>
+      <c r="J20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
         <v>24</v>
       </c>
-      <c r="B21" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" t="s">
-        <v>7</v>
+      <c r="B21" s="8">
+        <v>3</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2</v>
+      </c>
+      <c r="D21" s="8">
+        <v>3</v>
+      </c>
+      <c r="E21" s="8">
+        <v>4</v>
+      </c>
+      <c r="F21" s="8">
+        <v>3</v>
+      </c>
+      <c r="G21" s="8">
+        <v>4</v>
+      </c>
+      <c r="H21" s="8">
+        <v>3</v>
+      </c>
+      <c r="I21" s="8">
+        <v>4</v>
+      </c>
+      <c r="J21" s="8">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -3605,452 +3386,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843227C6-68DD-47EB-9A6D-734AD66A81DC}">
-  <dimension ref="A1:F21"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:F21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6">
-        <v>7</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
-        <v>7</v>
-      </c>
-      <c r="F3" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>6</v>
-      </c>
-      <c r="F4" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6">
-        <v>7</v>
-      </c>
-      <c r="F5" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
-        <v>6</v>
-      </c>
-      <c r="F6" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6">
-        <v>2</v>
-      </c>
-      <c r="E7" s="6">
-        <v>6</v>
-      </c>
-      <c r="F7" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>12</v>
-      </c>
-      <c r="B9" s="6">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6">
-        <v>7</v>
-      </c>
-      <c r="D9" s="6">
-        <v>2</v>
-      </c>
-      <c r="E9" s="6">
-        <v>7</v>
-      </c>
-      <c r="F9" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>14</v>
-      </c>
-      <c r="B11" s="6">
-        <v>6</v>
-      </c>
-      <c r="C11" s="6">
-        <v>6</v>
-      </c>
-      <c r="D11" s="6">
-        <v>2</v>
-      </c>
-      <c r="E11" s="6">
-        <v>6</v>
-      </c>
-      <c r="F11" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>15</v>
-      </c>
-      <c r="B12" s="4">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4">
-        <v>5</v>
-      </c>
-      <c r="F12" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>16</v>
-      </c>
-      <c r="B13" s="6">
-        <v>7</v>
-      </c>
-      <c r="C13" s="6">
-        <v>7</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
-        <v>5</v>
-      </c>
-      <c r="F13" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>17</v>
-      </c>
-      <c r="B14" s="4">
-        <v>6</v>
-      </c>
-      <c r="C14" s="4">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4">
-        <v>6</v>
-      </c>
-      <c r="F14" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
-        <v>18</v>
-      </c>
-      <c r="B15" s="6">
-        <v>7</v>
-      </c>
-      <c r="C15" s="6">
-        <v>7</v>
-      </c>
-      <c r="D15" s="6">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6">
-        <v>7</v>
-      </c>
-      <c r="F15" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>19</v>
-      </c>
-      <c r="B16" s="4">
-        <v>7</v>
-      </c>
-      <c r="C16" s="4">
-        <v>7</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4">
-        <v>7</v>
-      </c>
-      <c r="F16" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6">
-        <v>6</v>
-      </c>
-      <c r="C17" s="6">
-        <v>6</v>
-      </c>
-      <c r="D17" s="6">
-        <v>2</v>
-      </c>
-      <c r="E17" s="6">
-        <v>6</v>
-      </c>
-      <c r="F17" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>21</v>
-      </c>
-      <c r="B18" s="4">
-        <v>7</v>
-      </c>
-      <c r="C18" s="4">
-        <v>7</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4">
-        <v>7</v>
-      </c>
-      <c r="F18" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
-        <v>22</v>
-      </c>
-      <c r="B19" s="6">
-        <v>7</v>
-      </c>
-      <c r="C19" s="6">
-        <v>7</v>
-      </c>
-      <c r="D19" s="6">
-        <v>2</v>
-      </c>
-      <c r="E19" s="6">
-        <v>6</v>
-      </c>
-      <c r="F19" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>23</v>
-      </c>
-      <c r="B20" s="4">
-        <v>7</v>
-      </c>
-      <c r="C20" s="4">
-        <v>7</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4">
-        <v>7</v>
-      </c>
-      <c r="F20" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
-        <v>24</v>
-      </c>
-      <c r="B21" s="8">
-        <v>7</v>
-      </c>
-      <c r="C21" s="8">
-        <v>7</v>
-      </c>
-      <c r="D21" s="8">
-        <v>1</v>
-      </c>
-      <c r="E21" s="8">
-        <v>7</v>
-      </c>
-      <c r="F21" s="8">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78F1E53-17CB-42E3-8347-5D8F8BB9FD7F}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -4069,7 +3404,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4083,7 +3418,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4127,7 +3462,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4201,7 +3536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AED07B-BBCA-44A7-9642-D841C66484E7}">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -4226,25 +3561,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>137</v>
+        <v>76</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>139</v>
+        <v>78</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>143</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -4775,7 +4110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9620FC97-BB34-4AA1-9779-D683C787D662}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -4794,7 +4129,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4808,7 +4143,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4834,7 +4169,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4854,7 +4189,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4928,7 +4263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F4C1AA-3CEC-4795-ADE9-2F6C9E063DFC}">
   <dimension ref="A1:E21"/>
   <sheetViews>
@@ -4950,16 +4285,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -5310,7 +4645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FD4FC9-D492-4A3E-A816-59D059884F35}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -5329,7 +4664,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5343,7 +4678,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5387,7 +4722,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5461,7 +4796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7C77B0-DC6E-4904-A2E7-AB96C27ADC63}">
   <dimension ref="A1:G21"/>
   <sheetViews>
@@ -5485,22 +4820,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>149</v>
+        <v>88</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>153</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5969,7 +5304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B51B786-8F7D-4AE1-ACB4-9021B45B2B22}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -5988,7 +5323,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6002,7 +5337,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -6046,7 +5381,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -6120,7 +5455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF398F5B-1061-4739-AC99-3EE06740DCE0}">
   <dimension ref="A1:E21"/>
   <sheetViews>
@@ -6142,16 +5477,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>155</v>
+        <v>94</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>156</v>
+        <v>95</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>157</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -6502,7 +5837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350CC601-5ED6-4586-8F65-2B5EA9A2217B}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -6521,7 +5856,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6535,7 +5870,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -6579,7 +5914,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -6653,711 +5988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21EFD8E-1233-4766-ABCE-33EC154D85E9}">
-  <dimension ref="A1:J21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" customWidth="1"/>
-    <col min="3" max="3" width="37.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="75.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="69.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="65.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4">
-        <v>4</v>
-      </c>
-      <c r="H2" s="4">
-        <v>4</v>
-      </c>
-      <c r="I2" s="4">
-        <v>4</v>
-      </c>
-      <c r="J2" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6">
-        <v>5</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6">
-        <v>4</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2</v>
-      </c>
-      <c r="F3" s="6">
-        <v>2</v>
-      </c>
-      <c r="G3" s="6">
-        <v>5</v>
-      </c>
-      <c r="H3" s="6">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6">
-        <v>5</v>
-      </c>
-      <c r="J3" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4">
-        <v>4</v>
-      </c>
-      <c r="F4" s="4">
-        <v>2</v>
-      </c>
-      <c r="G4" s="4">
-        <v>5</v>
-      </c>
-      <c r="H4" s="4">
-        <v>3</v>
-      </c>
-      <c r="I4" s="4">
-        <v>5</v>
-      </c>
-      <c r="J4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6">
-        <v>5</v>
-      </c>
-      <c r="C5" s="6">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6">
-        <v>2</v>
-      </c>
-      <c r="E5" s="6">
-        <v>5</v>
-      </c>
-      <c r="F5" s="6">
-        <v>4</v>
-      </c>
-      <c r="G5" s="6">
-        <v>4</v>
-      </c>
-      <c r="H5" s="6">
-        <v>4</v>
-      </c>
-      <c r="I5" s="6">
-        <v>4</v>
-      </c>
-      <c r="J5" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4">
-        <v>3</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
-        <v>5</v>
-      </c>
-      <c r="F6" s="4">
-        <v>4</v>
-      </c>
-      <c r="G6" s="4">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4">
-        <v>3</v>
-      </c>
-      <c r="I6" s="4">
-        <v>4</v>
-      </c>
-      <c r="J6" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6">
-        <v>4</v>
-      </c>
-      <c r="C7" s="6">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6">
-        <v>4</v>
-      </c>
-      <c r="E7" s="6">
-        <v>4</v>
-      </c>
-      <c r="F7" s="6">
-        <v>3</v>
-      </c>
-      <c r="G7" s="6">
-        <v>4</v>
-      </c>
-      <c r="H7" s="6">
-        <v>3</v>
-      </c>
-      <c r="I7" s="6">
-        <v>4</v>
-      </c>
-      <c r="J7" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2</v>
-      </c>
-      <c r="D8" s="4">
-        <v>4</v>
-      </c>
-      <c r="E8" s="4">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4">
-        <v>4</v>
-      </c>
-      <c r="G8" s="4">
-        <v>4</v>
-      </c>
-      <c r="H8" s="4">
-        <v>2</v>
-      </c>
-      <c r="I8" s="4">
-        <v>4</v>
-      </c>
-      <c r="J8" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>12</v>
-      </c>
-      <c r="B9" s="6">
-        <v>5</v>
-      </c>
-      <c r="C9" s="6">
-        <v>2</v>
-      </c>
-      <c r="D9" s="6">
-        <v>5</v>
-      </c>
-      <c r="E9" s="6">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6">
-        <v>2</v>
-      </c>
-      <c r="G9" s="6">
-        <v>5</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6">
-        <v>5</v>
-      </c>
-      <c r="J9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4">
-        <v>5</v>
-      </c>
-      <c r="F10" s="4">
-        <v>5</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4">
-        <v>5</v>
-      </c>
-      <c r="I10" s="4">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>14</v>
-      </c>
-      <c r="B11" s="6">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6">
-        <v>2</v>
-      </c>
-      <c r="D11" s="6">
-        <v>5</v>
-      </c>
-      <c r="E11" s="6">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6">
-        <v>4</v>
-      </c>
-      <c r="G11" s="6">
-        <v>5</v>
-      </c>
-      <c r="H11" s="6">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6">
-        <v>5</v>
-      </c>
-      <c r="J11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>15</v>
-      </c>
-      <c r="B12" s="4">
-        <v>4</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2</v>
-      </c>
-      <c r="D12" s="4">
-        <v>3</v>
-      </c>
-      <c r="E12" s="4">
-        <v>2</v>
-      </c>
-      <c r="F12" s="4">
-        <v>4</v>
-      </c>
-      <c r="G12" s="4">
-        <v>5</v>
-      </c>
-      <c r="H12" s="4">
-        <v>2</v>
-      </c>
-      <c r="I12" s="4">
-        <v>4</v>
-      </c>
-      <c r="J12" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>16</v>
-      </c>
-      <c r="B13" s="6">
-        <v>4</v>
-      </c>
-      <c r="C13" s="6">
-        <v>2</v>
-      </c>
-      <c r="D13" s="6">
-        <v>4</v>
-      </c>
-      <c r="E13" s="6">
-        <v>4</v>
-      </c>
-      <c r="F13" s="6">
-        <v>5</v>
-      </c>
-      <c r="G13" s="6">
-        <v>4</v>
-      </c>
-      <c r="H13" s="6">
-        <v>2</v>
-      </c>
-      <c r="I13" s="6">
-        <v>4</v>
-      </c>
-      <c r="J13" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>17</v>
-      </c>
-      <c r="B14" s="4">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4">
-        <v>2</v>
-      </c>
-      <c r="F14" s="4">
-        <v>4</v>
-      </c>
-      <c r="G14" s="4">
-        <v>5</v>
-      </c>
-      <c r="H14" s="4">
-        <v>4</v>
-      </c>
-      <c r="I14" s="4">
-        <v>4</v>
-      </c>
-      <c r="J14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
-        <v>18</v>
-      </c>
-      <c r="B15" s="6">
-        <v>2</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6">
-        <v>2</v>
-      </c>
-      <c r="E15" s="6">
-        <v>2</v>
-      </c>
-      <c r="F15" s="6">
-        <v>5</v>
-      </c>
-      <c r="G15" s="6">
-        <v>4</v>
-      </c>
-      <c r="H15" s="6">
-        <v>4</v>
-      </c>
-      <c r="I15" s="6">
-        <v>4</v>
-      </c>
-      <c r="J15" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>19</v>
-      </c>
-      <c r="B16" s="4">
-        <v>5</v>
-      </c>
-      <c r="C16" s="4">
-        <v>2</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4">
-        <v>3</v>
-      </c>
-      <c r="F16" s="4">
-        <v>4</v>
-      </c>
-      <c r="G16" s="4">
-        <v>4</v>
-      </c>
-      <c r="H16" s="4">
-        <v>3</v>
-      </c>
-      <c r="I16" s="4">
-        <v>5</v>
-      </c>
-      <c r="J16" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6">
-        <v>5</v>
-      </c>
-      <c r="D17" s="6">
-        <v>2</v>
-      </c>
-      <c r="E17" s="6">
-        <v>2</v>
-      </c>
-      <c r="F17" s="6">
-        <v>4</v>
-      </c>
-      <c r="G17" s="6">
-        <v>3</v>
-      </c>
-      <c r="H17" s="6">
-        <v>2</v>
-      </c>
-      <c r="I17" s="6">
-        <v>4</v>
-      </c>
-      <c r="J17" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>21</v>
-      </c>
-      <c r="B18" s="4">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4">
-        <v>2</v>
-      </c>
-      <c r="D18" s="4">
-        <v>4</v>
-      </c>
-      <c r="E18" s="4">
-        <v>5</v>
-      </c>
-      <c r="F18" s="4">
-        <v>3</v>
-      </c>
-      <c r="G18" s="4">
-        <v>4</v>
-      </c>
-      <c r="H18" s="4">
-        <v>3</v>
-      </c>
-      <c r="I18" s="4">
-        <v>3</v>
-      </c>
-      <c r="J18" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
-        <v>22</v>
-      </c>
-      <c r="B19" s="6">
-        <v>4</v>
-      </c>
-      <c r="C19" s="6">
-        <v>3</v>
-      </c>
-      <c r="D19" s="6">
-        <v>4</v>
-      </c>
-      <c r="E19" s="6">
-        <v>4</v>
-      </c>
-      <c r="F19" s="6">
-        <v>3</v>
-      </c>
-      <c r="G19" s="6">
-        <v>4</v>
-      </c>
-      <c r="H19" s="6">
-        <v>2</v>
-      </c>
-      <c r="I19" s="6">
-        <v>4</v>
-      </c>
-      <c r="J19" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>23</v>
-      </c>
-      <c r="B20" s="4">
-        <v>5</v>
-      </c>
-      <c r="C20" s="4">
-        <v>2</v>
-      </c>
-      <c r="D20" s="4">
-        <v>4</v>
-      </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="4">
-        <v>4</v>
-      </c>
-      <c r="G20" s="4">
-        <v>4</v>
-      </c>
-      <c r="H20" s="4">
-        <v>2</v>
-      </c>
-      <c r="I20" s="4">
-        <v>4</v>
-      </c>
-      <c r="J20" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
-        <v>24</v>
-      </c>
-      <c r="B21" s="8">
-        <v>3</v>
-      </c>
-      <c r="C21" s="8">
-        <v>2</v>
-      </c>
-      <c r="D21" s="8">
-        <v>3</v>
-      </c>
-      <c r="E21" s="8">
-        <v>4</v>
-      </c>
-      <c r="F21" s="8">
-        <v>3</v>
-      </c>
-      <c r="G21" s="8">
-        <v>4</v>
-      </c>
-      <c r="H21" s="8">
-        <v>3</v>
-      </c>
-      <c r="I21" s="8">
-        <v>4</v>
-      </c>
-      <c r="J21" s="8">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DB91FD-3F81-4EE6-8C43-DEB0EBE6AED0}">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -7378,13 +6009,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>158</v>
+        <v>97</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>159</v>
+        <v>98</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>160</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -7675,7 +6306,172 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AAF1C9C-A06D-4EA8-B0B6-7A53173E550A}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="161.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>16</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>18</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>20</v>
+      </c>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>21</v>
+      </c>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>22</v>
+      </c>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>23</v>
+      </c>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>24</v>
+      </c>
+      <c r="B21" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B503E080-426C-4E3E-9B13-574D03894FA5}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -7694,7 +6490,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -7708,7 +6504,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -7752,7 +6548,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -7820,7 +6616,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -7828,11 +6624,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274BC49A-BDFD-4393-99E0-623D8A06551C}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -7847,7 +6643,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -7855,7 +6651,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -7863,7 +6659,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -7901,7 +6697,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -7909,7 +6705,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -7917,7 +6713,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -7925,7 +6721,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -7988,171 +6784,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AAF1C9C-A06D-4EA8-B0B6-7A53173E550A}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="161.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>12</v>
-      </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>14</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>15</v>
-      </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>16</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>17</v>
-      </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>18</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>19</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>21</v>
-      </c>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>22</v>
-      </c>
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>23</v>
-      </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>24</v>
-      </c>
-      <c r="B21" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148DBB12-F972-4C55-96BA-CA4E8335D753}">
   <dimension ref="A1:L21"/>
   <sheetViews>
@@ -8181,37 +6812,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>108</v>
+        <v>47</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>112</v>
+        <v>51</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>114</v>
+        <v>53</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>115</v>
+        <v>54</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -8982,7 +7613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F56DC322-C8A8-4C06-85B7-D37F67F1446E}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -9001,7 +7632,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -9015,7 +7646,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -9059,7 +7690,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -9091,7 +7722,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -9135,7 +7766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0594A1-C3ED-4DCD-AAD7-56B2F951BD7C}">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -9160,25 +7791,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>119</v>
+        <v>58</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>120</v>
+        <v>59</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>121</v>
+        <v>60</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>122</v>
+        <v>61</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>123</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -9709,7 +8340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BAB1D7-7236-4775-A469-BA0EEDD3C87E}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -9728,7 +8359,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -9742,7 +8373,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -9768,7 +8399,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -9788,7 +8419,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -9820,7 +8451,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -9858,7 +8489,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -9866,7 +8497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6496DE57-341C-4351-915F-A89A0B4D0E6D}">
   <dimension ref="A1:I21"/>
   <sheetViews>
@@ -9892,28 +8523,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>126</v>
+        <v>65</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>127</v>
+        <v>66</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>130</v>
+        <v>69</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -10502,7 +9133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B820EA8F-FBB4-4F57-99FB-6ABC36D4605A}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -10521,7 +9152,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -10535,7 +9166,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -10561,7 +9192,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -10581,7 +9212,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -10601,7 +9232,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -10615,7 +9246,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -10647,7 +9278,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -10659,4 +9290,450 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843227C6-68DD-47EB-9A6D-734AD66A81DC}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>7</v>
+      </c>
+      <c r="F3" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>7</v>
+      </c>
+      <c r="F5" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>7</v>
+      </c>
+      <c r="F9" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2</v>
+      </c>
+      <c r="E11" s="6">
+        <v>6</v>
+      </c>
+      <c r="F11" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>16</v>
+      </c>
+      <c r="B13" s="6">
+        <v>7</v>
+      </c>
+      <c r="C13" s="6">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <v>5</v>
+      </c>
+      <c r="F13" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>18</v>
+      </c>
+      <c r="B15" s="6">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6">
+        <v>7</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6">
+        <v>7</v>
+      </c>
+      <c r="F15" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4">
+        <v>7</v>
+      </c>
+      <c r="C16" s="4">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>7</v>
+      </c>
+      <c r="F16" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>20</v>
+      </c>
+      <c r="B17" s="6">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6">
+        <v>6</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2</v>
+      </c>
+      <c r="E17" s="6">
+        <v>6</v>
+      </c>
+      <c r="F17" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>21</v>
+      </c>
+      <c r="B18" s="4">
+        <v>7</v>
+      </c>
+      <c r="C18" s="4">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <v>7</v>
+      </c>
+      <c r="F18" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>22</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7</v>
+      </c>
+      <c r="C19" s="6">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6">
+        <v>2</v>
+      </c>
+      <c r="E19" s="6">
+        <v>6</v>
+      </c>
+      <c r="F19" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>23</v>
+      </c>
+      <c r="B20" s="4">
+        <v>7</v>
+      </c>
+      <c r="C20" s="4">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>7</v>
+      </c>
+      <c r="F20" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>24</v>
+      </c>
+      <c r="B21" s="8">
+        <v>7</v>
+      </c>
+      <c r="C21" s="8">
+        <v>7</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+      <c r="E21" s="8">
+        <v>7</v>
+      </c>
+      <c r="F21" s="8">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>